<commit_message>
sheet updates and new column addition to the script.
</commit_message>
<xml_diff>
--- a/projects/oc/sch_test.xlsx
+++ b/projects/oc/sch_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -40,58 +40,169 @@
     <t xml:space="preserve">D2</t>
   </si>
   <si>
-    <t xml:space="preserve">string1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dstring9</t>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e9</t>
   </si>
 </sst>
 </file>
@@ -303,10 +414,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -330,25 +441,31 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>45485</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,19 +473,22 @@
         <v>45486</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,19 +496,22 @@
         <v>45487</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,19 +519,22 @@
         <v>45488</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,19 +542,22 @@
         <v>45489</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,19 +565,22 @@
         <v>45490</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,19 +588,22 @@
         <v>45491</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,19 +611,22 @@
         <v>45492</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,19 +634,22 @@
         <v>45493</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>59</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>